<commit_message>
final mods and more recs 2
</commit_message>
<xml_diff>
--- a/docs/model_outcomes.xlsx
+++ b/docs/model_outcomes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrischan/Documents/02_Class/Metis/bootcamp/githubrepo/Metis_proj2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB917CD5-DECD-614A-9414-6BBC7C928D39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7F2C4B-BC06-314E-8FF9-CF21F63B1A6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2500" windowWidth="26440" windowHeight="14940" xr2:uid="{4703248F-0375-9844-9362-62B8AFC2E45D}"/>
+    <workbookView xWindow="4400" yWindow="4440" windowWidth="21660" windowHeight="15900" xr2:uid="{4703248F-0375-9844-9362-62B8AFC2E45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Model</t>
   </si>
@@ -95,13 +96,55 @@
   </si>
   <si>
     <t>Ridge CV poly+Standard</t>
+  </si>
+  <si>
+    <t>Lasso Test</t>
+  </si>
+  <si>
+    <t>Ridge Test</t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Record Label</t>
+  </si>
+  <si>
+    <t>Album Ratings</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Haves</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Sleeve Grade</t>
+  </si>
+  <si>
+    <t>Wants</t>
+  </si>
+  <si>
+    <t>Seller Rating</t>
+  </si>
+  <si>
+    <t>Media Grade</t>
+  </si>
+  <si>
+    <t>Release Date</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,16 +152,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Next Regular"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,11 +200,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -138,9 +228,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,13 +564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7878247-AC21-9E42-B57C-B7C974DCF01A}">
-  <dimension ref="B3:G10"/>
+  <dimension ref="B3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -467,7 +579,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="51">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -507,27 +619,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="1">
+    <row r="5" spans="2:7">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>0.20599999999999999</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>61.95</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>114.125</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -535,19 +647,19 @@
         <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>0.22500000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="E6" s="1">
-        <v>63.764000000000003</v>
+        <v>63.689</v>
       </c>
       <c r="F6" s="1">
-        <v>131.12799999999999</v>
+        <v>130.46199999999999</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -561,58 +673,191 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="D8" s="5">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="E9" s="1">
-        <v>52.783999999999999</v>
-      </c>
-      <c r="F9" s="1">
-        <v>125.185</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="D9" s="5">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E9" s="5">
+        <v>52.966000000000001</v>
+      </c>
+      <c r="F9" s="5">
+        <v>125.69799999999999</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7">
       <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.39329999999999998</v>
-      </c>
-      <c r="E10" s="1">
-        <v>52.85</v>
-      </c>
-      <c r="F10" s="1">
-        <v>119.49</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="D10" s="5">
+        <v>0.41689999999999999</v>
+      </c>
+      <c r="E10" s="5">
+        <v>52.79</v>
+      </c>
+      <c r="F10" s="5">
+        <v>118.28</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.35260000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.35770000000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>52.112000000000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>111.89</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9">
+      <c r="I17" s="1">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9">
+      <c r="I19" s="4">
+        <f>(I17-I18)/I18</f>
+        <v>4.9166666666666661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF669CA-96DC-EA4B-A760-15585E6B52DE}">
+  <dimension ref="E5:K9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="31" customHeight="1"/>
+  <cols>
+    <col min="5" max="5" width="12.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:11" ht="38" customHeight="1">
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="5:11" ht="20" customHeight="1">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="5:11" ht="38" customHeight="1">
+      <c r="E7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" ht="20" customHeight="1">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="5:11" ht="38" customHeight="1">
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>